<commit_message>
Chưa xử lý chấm công cho toàn bộ data
</commit_message>
<xml_diff>
--- a/ChamCongTuan/HoSoNhanSu.xlsx
+++ b/ChamCongTuan/HoSoNhanSu.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://poxz-my.sharepoint.com/personal/buuduc1999_poxz_onmicrosoft_com/Documents/User/ADMIN/Desktop/ChamCongTuan/ChamCongTuan/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OneDrive - poxz\User\ADMIN\Documents\GitHub\ChamCongTuan\ChamCongTuan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{6DED4DEE-1466-4FBD-9A00-1416623C3A8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00BFE95B-B69A-44D3-9122-65C335BF437E}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{6DED4DEE-1466-4FBD-9A00-1416623C3A8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1F326ECD-9B69-4D0F-A412-809C79157A3C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{10EE1D37-D4C0-4203-A77A-ABF6365B953C}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{10EE1D37-D4C0-4203-A77A-ABF6365B953C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1050,10 +1051,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1372,7 +1373,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE48DB8B-7BB4-4914-B895-64CB6A0C3747}">
   <dimension ref="A1:F86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -1388,13 +1389,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -3099,7 +3100,1029 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E91F9EC-9384-430D-B90B-6E9B290A8DBB}">
+  <dimension ref="A1:S22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1">
+        <v>3</v>
+      </c>
+      <c r="D1">
+        <v>4</v>
+      </c>
+      <c r="E1">
+        <v>5</v>
+      </c>
+      <c r="F1">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>7</v>
+      </c>
+      <c r="H1">
+        <v>8</v>
+      </c>
+      <c r="I1">
+        <v>9</v>
+      </c>
+      <c r="J1">
+        <v>10</v>
+      </c>
+      <c r="K1">
+        <v>11</v>
+      </c>
+      <c r="L1">
+        <v>12</v>
+      </c>
+      <c r="M1">
+        <v>13</v>
+      </c>
+      <c r="N1">
+        <v>14</v>
+      </c>
+      <c r="O1">
+        <v>15</v>
+      </c>
+      <c r="P1">
+        <v>16</v>
+      </c>
+      <c r="Q1">
+        <v>17</v>
+      </c>
+      <c r="R1">
+        <v>18</v>
+      </c>
+      <c r="S1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+      <c r="M2">
+        <v>2</v>
+      </c>
+      <c r="O2">
+        <v>2</v>
+      </c>
+      <c r="Q2">
+        <v>2</v>
+      </c>
+      <c r="S2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>-1</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
+      <c r="G3">
+        <v>-3</v>
+      </c>
+      <c r="H3">
+        <v>8</v>
+      </c>
+      <c r="I3">
+        <v>-5</v>
+      </c>
+      <c r="J3">
+        <v>10</v>
+      </c>
+      <c r="K3">
+        <v>-7</v>
+      </c>
+      <c r="L3">
+        <v>12</v>
+      </c>
+      <c r="M3">
+        <v>-9</v>
+      </c>
+      <c r="N3">
+        <v>14</v>
+      </c>
+      <c r="O3">
+        <v>-11</v>
+      </c>
+      <c r="P3">
+        <v>16</v>
+      </c>
+      <c r="Q3">
+        <v>-13</v>
+      </c>
+      <c r="R3">
+        <v>18</v>
+      </c>
+      <c r="S3">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>-4</v>
+      </c>
+      <c r="G4">
+        <v>-8</v>
+      </c>
+      <c r="I4">
+        <v>-12</v>
+      </c>
+      <c r="K4">
+        <v>-16</v>
+      </c>
+      <c r="M4">
+        <v>-20</v>
+      </c>
+      <c r="O4">
+        <v>-24</v>
+      </c>
+      <c r="Q4">
+        <v>-28</v>
+      </c>
+      <c r="S4">
+        <v>-32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>-1</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>-7</v>
+      </c>
+      <c r="F5">
+        <v>6</v>
+      </c>
+      <c r="G5">
+        <v>-13</v>
+      </c>
+      <c r="H5">
+        <v>8</v>
+      </c>
+      <c r="I5">
+        <v>-19</v>
+      </c>
+      <c r="J5">
+        <v>10</v>
+      </c>
+      <c r="K5">
+        <v>-25</v>
+      </c>
+      <c r="L5">
+        <v>12</v>
+      </c>
+      <c r="M5">
+        <v>-31</v>
+      </c>
+      <c r="N5">
+        <v>14</v>
+      </c>
+      <c r="O5">
+        <v>-37</v>
+      </c>
+      <c r="P5">
+        <v>16</v>
+      </c>
+      <c r="Q5">
+        <v>-43</v>
+      </c>
+      <c r="R5">
+        <v>18</v>
+      </c>
+      <c r="S5">
+        <v>-49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>-2</v>
+      </c>
+      <c r="E6">
+        <v>-10</v>
+      </c>
+      <c r="G6">
+        <v>-18</v>
+      </c>
+      <c r="I6">
+        <v>-26</v>
+      </c>
+      <c r="K6">
+        <v>-34</v>
+      </c>
+      <c r="M6">
+        <v>-42</v>
+      </c>
+      <c r="O6">
+        <v>-50</v>
+      </c>
+      <c r="Q6">
+        <v>-58</v>
+      </c>
+      <c r="S6">
+        <v>-66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>-3</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>-13</v>
+      </c>
+      <c r="F7">
+        <v>6</v>
+      </c>
+      <c r="G7">
+        <v>-23</v>
+      </c>
+      <c r="H7">
+        <v>8</v>
+      </c>
+      <c r="I7">
+        <v>-33</v>
+      </c>
+      <c r="J7">
+        <v>10</v>
+      </c>
+      <c r="K7">
+        <v>-43</v>
+      </c>
+      <c r="L7">
+        <v>12</v>
+      </c>
+      <c r="M7">
+        <v>-53</v>
+      </c>
+      <c r="N7">
+        <v>14</v>
+      </c>
+      <c r="O7">
+        <v>-63</v>
+      </c>
+      <c r="P7">
+        <v>16</v>
+      </c>
+      <c r="Q7">
+        <v>-73</v>
+      </c>
+      <c r="R7">
+        <v>18</v>
+      </c>
+      <c r="S7">
+        <v>-83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>-4</v>
+      </c>
+      <c r="E8">
+        <v>-16</v>
+      </c>
+      <c r="G8">
+        <v>-28</v>
+      </c>
+      <c r="I8">
+        <v>-40</v>
+      </c>
+      <c r="K8">
+        <v>-52</v>
+      </c>
+      <c r="M8">
+        <v>-64</v>
+      </c>
+      <c r="O8">
+        <v>-76</v>
+      </c>
+      <c r="Q8">
+        <v>-88</v>
+      </c>
+      <c r="S8">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>-5</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>-19</v>
+      </c>
+      <c r="F9">
+        <v>6</v>
+      </c>
+      <c r="G9">
+        <v>-33</v>
+      </c>
+      <c r="H9">
+        <v>8</v>
+      </c>
+      <c r="I9">
+        <v>-47</v>
+      </c>
+      <c r="J9">
+        <v>10</v>
+      </c>
+      <c r="K9">
+        <v>-61</v>
+      </c>
+      <c r="L9">
+        <v>12</v>
+      </c>
+      <c r="M9">
+        <v>-75</v>
+      </c>
+      <c r="N9">
+        <v>14</v>
+      </c>
+      <c r="O9">
+        <v>-89</v>
+      </c>
+      <c r="P9">
+        <v>16</v>
+      </c>
+      <c r="Q9">
+        <v>-103</v>
+      </c>
+      <c r="R9">
+        <v>18</v>
+      </c>
+      <c r="S9">
+        <v>-117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>-6</v>
+      </c>
+      <c r="E10">
+        <v>-22</v>
+      </c>
+      <c r="G10">
+        <v>-38</v>
+      </c>
+      <c r="I10">
+        <v>-54</v>
+      </c>
+      <c r="K10">
+        <v>-70</v>
+      </c>
+      <c r="M10">
+        <v>-86</v>
+      </c>
+      <c r="O10">
+        <v>-102</v>
+      </c>
+      <c r="Q10">
+        <v>-118</v>
+      </c>
+      <c r="S10">
+        <v>-134</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>-7</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>-25</v>
+      </c>
+      <c r="F11">
+        <v>6</v>
+      </c>
+      <c r="G11">
+        <v>-43</v>
+      </c>
+      <c r="H11">
+        <v>8</v>
+      </c>
+      <c r="I11">
+        <v>-61</v>
+      </c>
+      <c r="J11">
+        <v>10</v>
+      </c>
+      <c r="K11">
+        <v>-79</v>
+      </c>
+      <c r="L11">
+        <v>12</v>
+      </c>
+      <c r="M11">
+        <v>-97</v>
+      </c>
+      <c r="N11">
+        <v>14</v>
+      </c>
+      <c r="O11">
+        <v>-115</v>
+      </c>
+      <c r="P11">
+        <v>16</v>
+      </c>
+      <c r="Q11">
+        <v>-133</v>
+      </c>
+      <c r="R11">
+        <v>18</v>
+      </c>
+      <c r="S11">
+        <v>-151</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>-8</v>
+      </c>
+      <c r="E12">
+        <v>-28</v>
+      </c>
+      <c r="G12">
+        <v>-48</v>
+      </c>
+      <c r="I12">
+        <v>-68</v>
+      </c>
+      <c r="K12">
+        <v>-88</v>
+      </c>
+      <c r="M12">
+        <v>-108</v>
+      </c>
+      <c r="O12">
+        <v>-128</v>
+      </c>
+      <c r="Q12">
+        <v>-148</v>
+      </c>
+      <c r="S12">
+        <v>-168</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>-9</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>-31</v>
+      </c>
+      <c r="F13">
+        <v>6</v>
+      </c>
+      <c r="G13">
+        <v>-53</v>
+      </c>
+      <c r="H13">
+        <v>8</v>
+      </c>
+      <c r="I13">
+        <v>-75</v>
+      </c>
+      <c r="J13">
+        <v>10</v>
+      </c>
+      <c r="K13">
+        <v>-97</v>
+      </c>
+      <c r="L13">
+        <v>12</v>
+      </c>
+      <c r="M13">
+        <v>-119</v>
+      </c>
+      <c r="N13">
+        <v>14</v>
+      </c>
+      <c r="O13">
+        <v>-141</v>
+      </c>
+      <c r="P13">
+        <v>16</v>
+      </c>
+      <c r="Q13">
+        <v>-163</v>
+      </c>
+      <c r="R13">
+        <v>18</v>
+      </c>
+      <c r="S13">
+        <v>-185</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>-10</v>
+      </c>
+      <c r="E14">
+        <v>-34</v>
+      </c>
+      <c r="G14">
+        <v>-58</v>
+      </c>
+      <c r="I14">
+        <v>-82</v>
+      </c>
+      <c r="K14">
+        <v>-106</v>
+      </c>
+      <c r="M14">
+        <v>-130</v>
+      </c>
+      <c r="O14">
+        <v>-154</v>
+      </c>
+      <c r="Q14">
+        <v>-178</v>
+      </c>
+      <c r="S14">
+        <v>-202</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>-11</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <v>-37</v>
+      </c>
+      <c r="F15">
+        <v>6</v>
+      </c>
+      <c r="G15">
+        <v>-63</v>
+      </c>
+      <c r="H15">
+        <v>8</v>
+      </c>
+      <c r="I15">
+        <v>-89</v>
+      </c>
+      <c r="J15">
+        <v>10</v>
+      </c>
+      <c r="K15">
+        <v>-115</v>
+      </c>
+      <c r="L15">
+        <v>12</v>
+      </c>
+      <c r="M15">
+        <v>-141</v>
+      </c>
+      <c r="N15">
+        <v>14</v>
+      </c>
+      <c r="O15">
+        <v>-167</v>
+      </c>
+      <c r="P15">
+        <v>16</v>
+      </c>
+      <c r="Q15">
+        <v>-193</v>
+      </c>
+      <c r="R15">
+        <v>18</v>
+      </c>
+      <c r="S15">
+        <v>-219</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="C16">
+        <v>-12</v>
+      </c>
+      <c r="E16">
+        <v>-40</v>
+      </c>
+      <c r="G16">
+        <v>-68</v>
+      </c>
+      <c r="I16">
+        <v>-96</v>
+      </c>
+      <c r="K16">
+        <v>-124</v>
+      </c>
+      <c r="M16">
+        <v>-152</v>
+      </c>
+      <c r="O16">
+        <v>-180</v>
+      </c>
+      <c r="Q16">
+        <v>-208</v>
+      </c>
+      <c r="S16">
+        <v>-236</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>-13</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17">
+        <v>-43</v>
+      </c>
+      <c r="F17">
+        <v>6</v>
+      </c>
+      <c r="G17">
+        <v>-73</v>
+      </c>
+      <c r="H17">
+        <v>8</v>
+      </c>
+      <c r="I17">
+        <v>-103</v>
+      </c>
+      <c r="J17">
+        <v>10</v>
+      </c>
+      <c r="K17">
+        <v>-133</v>
+      </c>
+      <c r="L17">
+        <v>12</v>
+      </c>
+      <c r="M17">
+        <v>-163</v>
+      </c>
+      <c r="N17">
+        <v>14</v>
+      </c>
+      <c r="O17">
+        <v>-193</v>
+      </c>
+      <c r="P17">
+        <v>16</v>
+      </c>
+      <c r="Q17">
+        <v>-223</v>
+      </c>
+      <c r="R17">
+        <v>18</v>
+      </c>
+      <c r="S17">
+        <v>-253</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="C18">
+        <v>-14</v>
+      </c>
+      <c r="E18">
+        <v>-46</v>
+      </c>
+      <c r="G18">
+        <v>-78</v>
+      </c>
+      <c r="I18">
+        <v>-110</v>
+      </c>
+      <c r="K18">
+        <v>-142</v>
+      </c>
+      <c r="M18">
+        <v>-174</v>
+      </c>
+      <c r="O18">
+        <v>-206</v>
+      </c>
+      <c r="Q18">
+        <v>-238</v>
+      </c>
+      <c r="S18">
+        <v>-270</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>-15</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+      <c r="E19">
+        <v>-49</v>
+      </c>
+      <c r="F19">
+        <v>6</v>
+      </c>
+      <c r="G19">
+        <v>-83</v>
+      </c>
+      <c r="H19">
+        <v>8</v>
+      </c>
+      <c r="I19">
+        <v>-117</v>
+      </c>
+      <c r="J19">
+        <v>10</v>
+      </c>
+      <c r="K19">
+        <v>-151</v>
+      </c>
+      <c r="L19">
+        <v>12</v>
+      </c>
+      <c r="M19">
+        <v>-185</v>
+      </c>
+      <c r="N19">
+        <v>14</v>
+      </c>
+      <c r="O19">
+        <v>-219</v>
+      </c>
+      <c r="P19">
+        <v>16</v>
+      </c>
+      <c r="Q19">
+        <v>-253</v>
+      </c>
+      <c r="R19">
+        <v>18</v>
+      </c>
+      <c r="S19">
+        <v>-287</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="C20">
+        <v>-16</v>
+      </c>
+      <c r="E20">
+        <v>-52</v>
+      </c>
+      <c r="G20">
+        <v>-88</v>
+      </c>
+      <c r="I20">
+        <v>-124</v>
+      </c>
+      <c r="K20">
+        <v>-160</v>
+      </c>
+      <c r="M20">
+        <v>-196</v>
+      </c>
+      <c r="O20">
+        <v>-232</v>
+      </c>
+      <c r="Q20">
+        <v>-268</v>
+      </c>
+      <c r="S20">
+        <v>-304</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>-17</v>
+      </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
+      <c r="E21">
+        <v>-55</v>
+      </c>
+      <c r="F21">
+        <v>6</v>
+      </c>
+      <c r="G21">
+        <v>-93</v>
+      </c>
+      <c r="H21">
+        <v>8</v>
+      </c>
+      <c r="I21">
+        <v>-131</v>
+      </c>
+      <c r="J21">
+        <v>10</v>
+      </c>
+      <c r="K21">
+        <v>-169</v>
+      </c>
+      <c r="L21">
+        <v>12</v>
+      </c>
+      <c r="M21">
+        <v>-207</v>
+      </c>
+      <c r="N21">
+        <v>14</v>
+      </c>
+      <c r="O21">
+        <v>-245</v>
+      </c>
+      <c r="P21">
+        <v>16</v>
+      </c>
+      <c r="Q21">
+        <v>-283</v>
+      </c>
+      <c r="R21">
+        <v>18</v>
+      </c>
+      <c r="S21">
+        <v>-321</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="C22">
+        <v>-18</v>
+      </c>
+      <c r="E22">
+        <v>-58</v>
+      </c>
+      <c r="G22">
+        <v>-98</v>
+      </c>
+      <c r="I22">
+        <v>-138</v>
+      </c>
+      <c r="K22">
+        <v>-178</v>
+      </c>
+      <c r="M22">
+        <v>-218</v>
+      </c>
+      <c r="O22">
+        <v>-258</v>
+      </c>
+      <c r="Q22">
+        <v>-298</v>
+      </c>
+      <c r="S22">
+        <v>-338</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010072CB4A47BA35E543A9D323490A912876" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="771dd9f204b2b9a698d99049e2aa03b6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="41e9ce9d-7ae6-45ad-94f2-1488919f34f4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bde0812ebd7f85d6205a7339d212adca" ns3:_="">
     <xsd:import namespace="41e9ce9d-7ae6-45ad-94f2-1488919f34f4"/>
@@ -3283,7 +4306,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -3292,13 +4315,23 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B477DEF-9518-4FC3-98CB-27BB161C621A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="41e9ce9d-7ae6-45ad-94f2-1488919f34f4"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD2DA9DB-8B64-49AE-BBE2-7DE43A22EC9C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3316,26 +4349,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F261FDA-AF77-4D6F-8C52-EC24D3EACAB3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B477DEF-9518-4FC3-98CB-27BB161C621A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="41e9ce9d-7ae6-45ad-94f2-1488919f34f4"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>